<commit_message>
Add pictures creating Raspberry Pi OS 64bit SD card image
</commit_message>
<xml_diff>
--- a/draws/figures.xlsx
+++ b/draws/figures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\git\qemu-raspberrypi\draws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5708B7CC-9BF0-4581-8EAC-5FC5F778018B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA5C424-1D2B-4757-A3D4-A01BF7A305D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="4305" windowWidth="24240" windowHeight="16950" activeTab="1" xr2:uid="{4EEC4420-4819-4286-B07B-548E4F5D1C98}"/>
+    <workbookView xWindow="7110" yWindow="1965" windowWidth="24135" windowHeight="16950" activeTab="1" xr2:uid="{4EEC4420-4819-4286-B07B-548E4F5D1C98}"/>
   </bookViews>
   <sheets>
     <sheet name="draw1" sheetId="1" r:id="rId1"/>
@@ -7123,6 +7123,431 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="29" name="グループ化 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC483C60-55EC-CE68-883C-4649B40D2C5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="857250" y="21431250"/>
+          <a:ext cx="5153025" cy="6267450"/>
+          <a:chOff x="857250" y="21431250"/>
+          <a:chExt cx="5153025" cy="6267450"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="23" name="グループ化 22">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC6A21FA-63F9-6482-9AA6-0DFF181E165D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="857250" y="21431250"/>
+            <a:ext cx="5153025" cy="6267450"/>
+            <a:chOff x="857250" y="21431250"/>
+            <a:chExt cx="5153025" cy="6267450"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="11" name="図 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1921F369-A17B-7C80-171C-E05E507405FF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="857250" y="21431250"/>
+              <a:ext cx="5153025" cy="6267450"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="15" name="テキスト ボックス 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDEA8A47-9F4F-44EA-B47B-BB1ED35ABBC8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2047875" y="22326600"/>
+              <a:ext cx="960840" cy="280205"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>PiHostName</a:t>
+              </a:r>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="16" name="テキスト ボックス 15">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88876EE5-9E80-421B-BCA4-0B2ADFD8666D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2066925" y="23040975"/>
+              <a:ext cx="961225" cy="280205"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>PiUserName</a:t>
+              </a:r>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="19" name="正方形/長方形 18">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DF52233-8DAA-5A37-FDD2-267F7465C3B2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1219200" y="23879175"/>
+              <a:ext cx="1390650" cy="371475"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="15000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="20" name="テキスト ボックス 19">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30045067-60ED-467F-B5AF-4B5D5D559CA6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2571751" y="24003000"/>
+              <a:ext cx="1257300" cy="280205"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Clear</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t> Check Wi-Fi</a:t>
+              </a:r>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="25" name="直線コネクタ 24">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F279A2F-7211-E284-1737-B7CDA3ED3867}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2590800" y="26850975"/>
+            <a:ext cx="247650" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="28" name="テキスト ボックス 27">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF9C8C1D-5834-4F16-B709-72835D4203CD}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2743200" y="26460450"/>
+            <a:ext cx="1619250" cy="280205"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Set</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> us keyboard layout</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7442,8 +7867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F625DB4-D53A-42B3-A783-EDD42AD65FAD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="AT99" sqref="AT99"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="AN147" sqref="AN147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>